<commit_message>
Add capture of one cube in the samll problem used to calibrate the game review
</commit_message>
<xml_diff>
--- a/docs/game-review-scoring.xlsx
+++ b/docs/game-review-scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\pijersi-certu\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23223E10-9B92-454D-85B6-D8DCC7062242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6C3973-D57B-4746-AF9B-F308A93EE743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -295,11 +295,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6366,8 +6368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6380,28 +6382,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -6475,7 +6477,7 @@
       <c r="D3" s="12">
         <v>0.46165001844280101</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="15" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>